<commit_message>
Actualizado documento de entrega y Excel
</commit_message>
<xml_diff>
--- a/Entregas/Entrega 4/Informe/Listado de componentes.xlsx
+++ b/Entregas/Entrega 4/Informe/Listado de componentes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Resistencia 1k Ohm</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>Terminal para Housing</t>
+  </si>
+  <si>
+    <t>Componentes adicionales</t>
+  </si>
+  <si>
+    <t>PIC16F877A</t>
+  </si>
+  <si>
+    <t>MAX232</t>
+  </si>
+  <si>
+    <t>16x2 LCD</t>
+  </si>
+  <si>
+    <t>Sensor de Luz</t>
+  </si>
+  <si>
+    <t>Sensor de Sonidos</t>
+  </si>
+  <si>
+    <t>Pulsadores</t>
+  </si>
+  <si>
+    <t>Cable USB a Serial</t>
   </si>
 </sst>
 </file>
@@ -144,17 +168,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -197,14 +255,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla134" displayName="Tabla134" ref="A1:D24" totalsRowShown="0">
-  <autoFilter ref="A1:D24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla134" displayName="Tabla134" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Producto"/>
     <tableColumn id="2" name="Cantidad"/>
-    <tableColumn id="3" name="Precio" dataDxfId="1" dataCellStyle="Moneda"/>
-    <tableColumn id="4" name="Total" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="3" name="Precio" dataDxfId="7" dataCellStyle="Moneda"/>
+    <tableColumn id="4" name="Total" dataDxfId="6" dataCellStyle="Moneda">
       <calculatedColumnFormula>B2*C2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A28:D36" totalsRowCount="1">
+  <autoFilter ref="A28:D36"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Producto" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Cantidad" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Precio" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="4" name="Total" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Moneda">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM([Total])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -496,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -507,7 +581,7 @@
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -895,16 +969,170 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <f>SUM(D2:D24)</f>
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4583</v>
+      </c>
+      <c r="D29" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D30" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7668</v>
+      </c>
+      <c r="D31" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>7668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3934</v>
+      </c>
+      <c r="D32" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4900</v>
+      </c>
+      <c r="D33" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4900</v>
+      </c>
+      <c r="D35" s="2">
+        <f>Tabla1[[#This Row],[Cantidad]]*Tabla1[[#This Row],[Precio]]</f>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="3">
+        <f>SUM([Total])</f>
+        <v>27385</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="4">
+        <f>D25+Tabla1[[#Totals],[Total]]</f>
+        <v>31968</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>